<commit_message>
FIX: date sort, ADD: border
</commit_message>
<xml_diff>
--- a/docs/_data/list_course_excel.xlsx
+++ b/docs/_data/list_course_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\rnn-sda\docs\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0E8484-DB24-4782-9BF8-8497110DAD34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF61A70-E58A-4299-A1BB-91AB38313E5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0512C7F0-257B-40FB-BD86-A23063D6504B}"/>
   </bookViews>
@@ -331,6 +331,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -379,6 +382,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -699,7 +705,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +715,7 @@
     <col min="4" max="4" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -738,7 +744,7 @@
       <c r="F1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -776,8 +782,8 @@
       <c r="F2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="2">
-        <v>2017</v>
+      <c r="G2" s="5">
+        <v>42979</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>28</v>
@@ -808,8 +814,8 @@
       <c r="F3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="2">
-        <v>2017</v>
+      <c r="G3" s="5">
+        <v>43132</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>28</v>
@@ -840,8 +846,8 @@
       <c r="F4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="2">
-        <v>2018</v>
+      <c r="G4" s="5">
+        <v>43191</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>28</v>
@@ -872,8 +878,8 @@
       <c r="F5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="2">
-        <v>2018</v>
+      <c r="G5" s="5">
+        <v>43192</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>28</v>
@@ -904,8 +910,8 @@
       <c r="F6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="2">
-        <v>2018</v>
+      <c r="G6" s="5">
+        <v>43192</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>33</v>
@@ -936,8 +942,8 @@
       <c r="F7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="2">
-        <v>2018</v>
+      <c r="G7" s="5">
+        <v>43313</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>33</v>
@@ -968,8 +974,8 @@
       <c r="F8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="2">
-        <v>2018</v>
+      <c r="G8" s="5">
+        <v>43282</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>33</v>
@@ -1000,8 +1006,8 @@
       <c r="F9" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="2">
-        <v>2018</v>
+      <c r="G9" s="5">
+        <v>43374</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>28</v>
@@ -1032,8 +1038,8 @@
       <c r="F10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="2">
-        <v>2018</v>
+      <c r="G10" s="5">
+        <v>43374</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>33</v>
@@ -1064,8 +1070,8 @@
       <c r="F11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="2">
-        <v>2018</v>
+      <c r="G11" s="5">
+        <v>43374</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>33</v>
@@ -1096,8 +1102,8 @@
       <c r="F12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="2">
-        <v>2019</v>
+      <c r="G12" s="5">
+        <v>43806</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>33</v>
@@ -1125,8 +1131,8 @@
       <c r="F13" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="2">
-        <v>2018</v>
+      <c r="G13" s="5">
+        <v>43398</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>62</v>
@@ -1148,8 +1154,8 @@
       <c r="F14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="2">
-        <v>2019</v>
+      <c r="G14" s="5">
+        <v>43581</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>66</v>
@@ -1171,8 +1177,8 @@
       <c r="F15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="2">
-        <v>2019</v>
+      <c r="G15" s="5">
+        <v>43670</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>70</v>
@@ -1194,8 +1200,8 @@
       <c r="F16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="2">
-        <v>2019</v>
+      <c r="G16" s="5">
+        <v>43678</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>66</v>
@@ -1257,8 +1263,8 @@
       <c r="F19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="2">
-        <v>2020</v>
+      <c r="G19" s="5">
+        <v>43831</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>83</v>
@@ -1340,5 +1346,6 @@
     <hyperlink ref="K21" r:id="rId26" xr:uid="{FE9F74D1-1B25-4AC3-94B2-1C60F2F4D306}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>